<commit_message>
Drassige driehoek cross section simulated. Looks beautiful.
</commit_message>
<xml_diff>
--- a/Projects/DrasseDriehoek/cases/DSN_NW_ZO/DSN_NW_ZO.xlsx
+++ b/Projects/DrasseDriehoek/cases/DSN_NW_ZO/DSN_NW_ZO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/DrasseDriehoek/cases/DSN_NW_ZO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD51E0-B376-F548-99B8-C519DB5F0355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6CD6F1-B9DD-B940-96DB-03E83B65E581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -2024,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -11892,10 +11892,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A2" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11938,20 +11938,544 @@
         <v>0</v>
       </c>
       <c r="B3" s="15">
-        <v>45292</v>
+        <v>45658</v>
       </c>
       <c r="C3" s="10">
-        <f>DATE(2054,1,1)-DATE(2024,1,1)</f>
-        <v>10958</v>
+        <f>B4-B3</f>
+        <v>365</v>
       </c>
       <c r="D3" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="10">
         <v>1.25</v>
       </c>
       <c r="F3" s="10">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15">
+        <v>46023</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:C28" si="0">B5-B4</f>
+        <v>365</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15">
+        <v>46388</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D5" s="10">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15">
+        <v>46753</v>
+      </c>
+      <c r="C6" s="10">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15">
+        <v>47119</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D7" s="10">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15">
+        <v>47484</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D8" s="10">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15">
+        <v>47849</v>
+      </c>
+      <c r="C9" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D9" s="10">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15">
+        <v>48214</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15">
+        <v>48580</v>
+      </c>
+      <c r="C11" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="15">
+        <v>48945</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D12" s="10">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="15">
+        <v>49310</v>
+      </c>
+      <c r="C13" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D13" s="10">
+        <v>3</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="15">
+        <v>49675</v>
+      </c>
+      <c r="C14" s="10">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="D14" s="10">
+        <v>3</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="15">
+        <v>50041</v>
+      </c>
+      <c r="C15" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D15" s="10">
+        <v>3</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="15">
+        <v>50406</v>
+      </c>
+      <c r="C16" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="15">
+        <v>50771</v>
+      </c>
+      <c r="C17" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15">
+        <v>51136</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="D18" s="10">
+        <v>3</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="15">
+        <v>51502</v>
+      </c>
+      <c r="C19" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D19" s="10">
+        <v>3</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15">
+        <v>51867</v>
+      </c>
+      <c r="C20" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D20" s="10">
+        <v>3</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="15">
+        <v>52232</v>
+      </c>
+      <c r="C21" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D21" s="10">
+        <v>3</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15">
+        <v>52597</v>
+      </c>
+      <c r="C22" s="10">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="D22" s="10">
+        <v>3</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="15">
+        <v>52963</v>
+      </c>
+      <c r="C23" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D23" s="10">
+        <v>3</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="15">
+        <v>53328</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D24" s="10">
+        <v>3</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="15">
+        <v>53693</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D25" s="10">
+        <v>3</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="15">
+        <v>54058</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="0"/>
+        <v>366</v>
+      </c>
+      <c r="D26" s="10">
+        <v>3</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="15">
+        <v>54424</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="D27" s="10">
+        <v>3</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="15">
+        <v>54789</v>
+      </c>
+      <c r="C28" s="10">
+        <v>365</v>
+      </c>
+      <c r="D28" s="10">
+        <v>3</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11966,8 +12490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12022,7 +12546,7 @@
         <v>0.2</v>
       </c>
       <c r="F2" s="2">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>393</v>
@@ -12069,7 +12593,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -12099,7 +12623,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0.01</v>
@@ -12129,7 +12653,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>10</v>
@@ -12159,7 +12683,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0.01</v>
@@ -12189,7 +12713,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -12219,7 +12743,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0.01</v>
@@ -12249,7 +12773,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -12279,7 +12803,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0.01</v>
@@ -12309,7 +12833,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>5</v>

</xml_diff>